<commit_message>
ran all summary tables
</commit_message>
<xml_diff>
--- a/outputs/tax_share_sum.xlsx
+++ b/outputs/tax_share_sum.xlsx
@@ -8,20 +8,55 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edreiyu/Documents/Projects/vat_burden_analysis/outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{1E8BBEBE-098C-AC41-A740-A6B653ABAEF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04C2CA8A-CEF8-954E-AF15-AA0814D92AAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{EE8D4940-C3F8-D340-AF33-192918B31EA6}"/>
+    <workbookView xWindow="1340" yWindow="760" windowWidth="35960" windowHeight="19480" activeTab="2" xr2:uid="{EE8D4940-C3F8-D340-AF33-192918B31EA6}"/>
   </bookViews>
   <sheets>
     <sheet name="tax_share" sheetId="1" r:id="rId1"/>
-    <sheet name="main_summary" sheetId="2" r:id="rId2"/>
+    <sheet name="tax_share_bydecile" sheetId="5" r:id="rId2"/>
+    <sheet name="vat_paid_and_foregone" sheetId="6" r:id="rId3"/>
+    <sheet name="main_summary-xx" sheetId="2" r:id="rId4"/>
+    <sheet name="main_summary" sheetId="3" r:id="rId5"/>
+    <sheet name="exempt_by_category" sheetId="4" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={8C6BB57B-27B5-5A4F-8438-7F8706399291}</author>
+  </authors>
+  <commentList>
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{8C6BB57B-27B5-5A4F-8438-7F8706399291}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    total vat foregone / total expenditures</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="71">
   <si>
     <t>NPCINC</t>
   </si>
@@ -138,18 +173,115 @@
   </si>
   <si>
     <t>simple get the average ETR per decile / also check min and max of ETR range</t>
+  </si>
+  <si>
+    <t>Total monthly</t>
+  </si>
+  <si>
+    <t>Total annual</t>
+  </si>
+  <si>
+    <t>billions</t>
+  </si>
+  <si>
+    <t>sum_vat_etr</t>
+  </si>
+  <si>
+    <t>sum_vat_foregone_etr</t>
+  </si>
+  <si>
+    <t>food_exempt</t>
+  </si>
+  <si>
+    <t>housing_&amp;utilities_exempt</t>
+  </si>
+  <si>
+    <t>furnishings_&amp;maintenance_exempt</t>
+  </si>
+  <si>
+    <t>health_exempt</t>
+  </si>
+  <si>
+    <t>transport_exempt</t>
+  </si>
+  <si>
+    <t>recreation_exempt</t>
+  </si>
+  <si>
+    <t>education_exempt</t>
+  </si>
+  <si>
+    <t>insurance_&amp;financial_exempt</t>
+  </si>
+  <si>
+    <t>food_exempt_share</t>
+  </si>
+  <si>
+    <t>housing_&amp;utilities_exempt_share</t>
+  </si>
+  <si>
+    <t>furnishings_&amp;maintenance_exempt_share</t>
+  </si>
+  <si>
+    <t>health_exempt_share</t>
+  </si>
+  <si>
+    <t>transport_exempt_share</t>
+  </si>
+  <si>
+    <t>recreation_exempt_share</t>
+  </si>
+  <si>
+    <t>education_exempt_share</t>
+  </si>
+  <si>
+    <t>insurance_&amp;financial_exempt_share</t>
+  </si>
+  <si>
+    <t>the share of exempt food spending for the poorest decile is 40% of their total expenditures</t>
+  </si>
+  <si>
+    <t>in contrast, the share of exempt food spending for the richest decile is only 14% of their total expenditures</t>
+  </si>
+  <si>
+    <t>So the poor benefits more from vat exemption on food.</t>
+  </si>
+  <si>
+    <t>56% of total expenditures of poorest HH are exempt from VAT</t>
+  </si>
+  <si>
+    <t>NOTES</t>
+  </si>
+  <si>
+    <t>vatable_share_decile</t>
+  </si>
+  <si>
+    <t>exempt_share_decile</t>
+  </si>
+  <si>
+    <t>estimated_vat_paid</t>
+  </si>
+  <si>
+    <t>estimated_vat_foregone</t>
+  </si>
+  <si>
+    <t>effective_vat_rate</t>
+  </si>
+  <si>
+    <t>This is monthly</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -284,8 +416,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -465,8 +603,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -581,6 +725,47 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -628,7 +813,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -646,7 +831,41 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="33" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="33" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="21" builtinId="30" customBuiltin="1"/>
@@ -705,6 +924,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="EU" id="{5E0609C9-F47C-1240-A063-C18A34FDDA35}" userId="EU" providerId="None"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1022,12 +1247,20 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="K1" dT="2025-11-25T09:34:07.87" personId="{5E0609C9-F47C-1240-A063-C18A34FDDA35}" id="{8C6BB57B-27B5-5A4F-8438-7F8706399291}">
+    <text>total vat foregone / total expenditures</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05A3A3A6-21B0-C748-9C6F-D3C4321EDE44}">
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1040,13 +1273,24 @@
     <col min="14" max="14" width="17.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E1" s="3" t="s">
+    <row r="1" spans="1:14" s="4" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="5" t="s">
         <v>18</v>
       </c>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="6"/>
     </row>
     <row r="2" spans="1:14" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -1545,18 +1789,56 @@
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="J14" s="3" t="s">
+    <row r="14" spans="1:14" s="18" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="L14" s="3" t="s">
+      <c r="K14" s="19"/>
+      <c r="L14" s="19" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="H15" s="3" t="s">
+      <c r="M14" s="19"/>
+      <c r="N14" s="20"/>
+    </row>
+    <row r="15" spans="1:14" s="18" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19" t="s">
         <v>16</v>
       </c>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="20"/>
+    </row>
+    <row r="16" spans="1:14" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1564,15 +1846,1274 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E37FD776-7F29-1443-8F72-00AEDE6040D3}">
-  <dimension ref="A1:M20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FD4DD6E-9753-F443-8851-2FA8C38B9693}">
+  <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="13" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="17.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="15" width="11" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>2747642.50515944</v>
+      </c>
+      <c r="C2" s="3">
+        <v>32807166219.147499</v>
+      </c>
+      <c r="D2" s="3">
+        <v>29276373226.599098</v>
+      </c>
+      <c r="E2" s="3">
+        <v>12730887016.797501</v>
+      </c>
+      <c r="F2" s="3">
+        <v>16287403643.337299</v>
+      </c>
+      <c r="G2" s="3">
+        <v>29018290660.1348</v>
+      </c>
+      <c r="H2" s="2">
+        <v>43.871939825480901</v>
+      </c>
+      <c r="I2" s="2">
+        <v>56.128060174519</v>
+      </c>
+      <c r="J2" s="2">
+        <v>38.805201679891702</v>
+      </c>
+      <c r="K2" s="2">
+        <v>49.645871681021198</v>
+      </c>
+      <c r="L2" s="2">
+        <v>43.485191687715101</v>
+      </c>
+      <c r="M2" s="2">
+        <v>55.633269590030203</v>
+      </c>
+      <c r="N2" s="2">
+        <v>4.5101528767221497</v>
+      </c>
+      <c r="O2" s="2">
+        <v>5.5347405121886402</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2748295.6540946802</v>
+      </c>
+      <c r="C3" s="3">
+        <v>41822410674.936996</v>
+      </c>
+      <c r="D3" s="3">
+        <v>35426039310.566101</v>
+      </c>
+      <c r="E3" s="3">
+        <v>16171881744.9347</v>
+      </c>
+      <c r="F3" s="3">
+        <v>18893257154.780602</v>
+      </c>
+      <c r="G3" s="3">
+        <v>35065138899.715302</v>
+      </c>
+      <c r="H3" s="2">
+        <v>46.119542806277003</v>
+      </c>
+      <c r="I3" s="2">
+        <v>53.880457193722897</v>
+      </c>
+      <c r="J3" s="2">
+        <v>38.667980835992402</v>
+      </c>
+      <c r="K3" s="2">
+        <v>45.174959668460197</v>
+      </c>
+      <c r="L3" s="2">
+        <v>45.649703042336199</v>
+      </c>
+      <c r="M3" s="2">
+        <v>53.331553632487299</v>
+      </c>
+      <c r="N3" s="2">
+        <v>5.7291890877431797</v>
+      </c>
+      <c r="O3" s="2">
+        <v>6.4202544537869501</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>2747874.69444041</v>
+      </c>
+      <c r="C4" s="3">
+        <v>47728594014.963997</v>
+      </c>
+      <c r="D4" s="3">
+        <v>39497871055.729301</v>
+      </c>
+      <c r="E4" s="3">
+        <v>18492395560.589802</v>
+      </c>
+      <c r="F4" s="3">
+        <v>20558976669.909401</v>
+      </c>
+      <c r="G4" s="3">
+        <v>39051372230.499298</v>
+      </c>
+      <c r="H4" s="2">
+        <v>47.354022418057802</v>
+      </c>
+      <c r="I4" s="2">
+        <v>52.645977581942098</v>
+      </c>
+      <c r="J4" s="2">
+        <v>38.744899032207101</v>
+      </c>
+      <c r="K4" s="2">
+        <v>43.074758630986999</v>
+      </c>
+      <c r="L4" s="2">
+        <v>46.8187146960353</v>
+      </c>
+      <c r="M4" s="2">
+        <v>52.050847603664103</v>
+      </c>
+      <c r="N4" s="2">
+        <v>6.5512741512066697</v>
+      </c>
+      <c r="O4" s="2">
+        <v>6.9862946578742502</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>2747979.4784429399</v>
+      </c>
+      <c r="C5" s="3">
+        <v>55228987672.520798</v>
+      </c>
+      <c r="D5" s="3">
+        <v>44792749154.822098</v>
+      </c>
+      <c r="E5" s="3">
+        <v>21174220742.446899</v>
+      </c>
+      <c r="F5" s="3">
+        <v>23060388456.8377</v>
+      </c>
+      <c r="G5" s="3">
+        <v>44234609199.284698</v>
+      </c>
+      <c r="H5" s="2">
+        <v>47.867995503370103</v>
+      </c>
+      <c r="I5" s="2">
+        <v>52.132004496629797</v>
+      </c>
+      <c r="J5" s="2">
+        <v>38.338962263800802</v>
+      </c>
+      <c r="K5" s="2">
+        <v>41.754139318239503</v>
+      </c>
+      <c r="L5" s="2">
+        <v>47.271536447249801</v>
+      </c>
+      <c r="M5" s="2">
+        <v>51.4824137655215</v>
+      </c>
+      <c r="N5" s="2">
+        <v>7.5013604682763004</v>
+      </c>
+      <c r="O5" s="2">
+        <v>7.8363175011677102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>2747628.8515828899</v>
+      </c>
+      <c r="C6" s="3">
+        <v>62300009849.796898</v>
+      </c>
+      <c r="D6" s="3">
+        <v>49501029635.587097</v>
+      </c>
+      <c r="E6" s="3">
+        <v>23802239836.017101</v>
+      </c>
+      <c r="F6" s="3">
+        <v>25029174922.970699</v>
+      </c>
+      <c r="G6" s="3">
+        <v>48831414758.9879</v>
+      </c>
+      <c r="H6" s="2">
+        <v>48.743703113037597</v>
+      </c>
+      <c r="I6" s="2">
+        <v>51.256296886962197</v>
+      </c>
+      <c r="J6" s="2">
+        <v>38.205836392969204</v>
+      </c>
+      <c r="K6" s="2">
+        <v>40.175234295010902</v>
+      </c>
+      <c r="L6" s="2">
+        <v>48.084332813362899</v>
+      </c>
+      <c r="M6" s="2">
+        <v>50.5629379979136</v>
+      </c>
+      <c r="N6" s="2">
+        <v>8.43238498049665</v>
+      </c>
+      <c r="O6" s="2">
+        <v>8.5053450793239804</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>2748336.9317767601</v>
+      </c>
+      <c r="C7" s="3">
+        <v>70697712578.309692</v>
+      </c>
+      <c r="D7" s="3">
+        <v>54853430904.834999</v>
+      </c>
+      <c r="E7" s="3">
+        <v>26514380477.310398</v>
+      </c>
+      <c r="F7" s="3">
+        <v>27502940702.588501</v>
+      </c>
+      <c r="G7" s="3">
+        <v>54017321179.898903</v>
+      </c>
+      <c r="H7" s="2">
+        <v>49.084959968686903</v>
+      </c>
+      <c r="I7" s="2">
+        <v>50.915040031313097</v>
+      </c>
+      <c r="J7" s="2">
+        <v>37.503873195248303</v>
+      </c>
+      <c r="K7" s="2">
+        <v>38.902164864420897</v>
+      </c>
+      <c r="L7" s="2">
+        <v>48.336776824972098</v>
+      </c>
+      <c r="M7" s="2">
+        <v>50.138961681910502</v>
+      </c>
+      <c r="N7" s="2">
+        <v>9.39321111140681</v>
+      </c>
+      <c r="O7" s="2">
+        <v>9.3459733327851708</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>2747846.3569293302</v>
+      </c>
+      <c r="C8" s="3">
+        <v>80541995781.497406</v>
+      </c>
+      <c r="D8" s="3">
+        <v>60962714759.237099</v>
+      </c>
+      <c r="E8" s="3">
+        <v>29742875498.603001</v>
+      </c>
+      <c r="F8" s="3">
+        <v>30134718319.903301</v>
+      </c>
+      <c r="G8" s="3">
+        <v>59877593818.506302</v>
+      </c>
+      <c r="H8" s="2">
+        <v>49.672796787319001</v>
+      </c>
+      <c r="I8" s="2">
+        <v>50.327203212680899</v>
+      </c>
+      <c r="J8" s="2">
+        <v>36.928406367396803</v>
+      </c>
+      <c r="K8" s="2">
+        <v>37.414913831606398</v>
+      </c>
+      <c r="L8" s="2">
+        <v>48.788633537840099</v>
+      </c>
+      <c r="M8" s="2">
+        <v>49.431391693949003</v>
+      </c>
+      <c r="N8" s="2">
+        <v>10.5369653595243</v>
+      </c>
+      <c r="O8" s="2">
+        <v>10.240296732425501</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>2747984.4327531499</v>
+      </c>
+      <c r="C9" s="3">
+        <v>95316514865.332199</v>
+      </c>
+      <c r="D9" s="3">
+        <v>69592985603.748001</v>
+      </c>
+      <c r="E9" s="3">
+        <v>33989743428.753101</v>
+      </c>
+      <c r="F9" s="3">
+        <v>34113196809.400902</v>
+      </c>
+      <c r="G9" s="3">
+        <v>68102940238.154099</v>
+      </c>
+      <c r="H9" s="2">
+        <v>49.909362664654402</v>
+      </c>
+      <c r="I9" s="2">
+        <v>50.090637335345598</v>
+      </c>
+      <c r="J9" s="2">
+        <v>35.659868047814697</v>
+      </c>
+      <c r="K9" s="2">
+        <v>35.789387450430397</v>
+      </c>
+      <c r="L9" s="2">
+        <v>48.8407605075109</v>
+      </c>
+      <c r="M9" s="2">
+        <v>49.018153932403898</v>
+      </c>
+      <c r="N9" s="2">
+        <v>12.041497100867399</v>
+      </c>
+      <c r="O9" s="2">
+        <v>11.5922523021949</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <v>2748042.5822946099</v>
+      </c>
+      <c r="C10" s="3">
+        <v>117372854152.933</v>
+      </c>
+      <c r="D10" s="3">
+        <v>82061193028.969299</v>
+      </c>
+      <c r="E10" s="3">
+        <v>40088129768.291</v>
+      </c>
+      <c r="F10" s="3">
+        <v>39657623068.682297</v>
+      </c>
+      <c r="G10" s="3">
+        <v>79745752836.973297</v>
+      </c>
+      <c r="H10" s="2">
+        <v>50.269924531585197</v>
+      </c>
+      <c r="I10" s="2">
+        <v>49.730075468414697</v>
+      </c>
+      <c r="J10" s="2">
+        <v>34.154515588465898</v>
+      </c>
+      <c r="K10" s="2">
+        <v>33.7877300120943</v>
+      </c>
+      <c r="L10" s="2">
+        <v>48.851507379546597</v>
+      </c>
+      <c r="M10" s="2">
+        <v>48.326890707867697</v>
+      </c>
+      <c r="N10" s="2">
+        <v>14.2019635833945</v>
+      </c>
+      <c r="O10" s="2">
+        <v>13.4763439171676</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3">
+        <v>2748063.5193039002</v>
+      </c>
+      <c r="C11" s="3">
+        <v>205068163103.01001</v>
+      </c>
+      <c r="D11" s="3">
+        <v>124958992792.82401</v>
+      </c>
+      <c r="E11" s="3">
+        <v>59564986259.146202</v>
+      </c>
+      <c r="F11" s="3">
+        <v>59038151385.299301</v>
+      </c>
+      <c r="G11" s="3">
+        <v>118603137644.44501</v>
+      </c>
+      <c r="H11" s="2">
+        <v>50.222099888885801</v>
+      </c>
+      <c r="I11" s="2">
+        <v>49.7779001111141</v>
+      </c>
+      <c r="J11" s="2">
+        <v>29.046432833762299</v>
+      </c>
+      <c r="K11" s="2">
+        <v>28.7895256347729</v>
+      </c>
+      <c r="L11" s="2">
+        <v>47.667626737278198</v>
+      </c>
+      <c r="M11" s="2">
+        <v>47.246020527055002</v>
+      </c>
+      <c r="N11" s="2">
+        <v>21.102001280361801</v>
+      </c>
+      <c r="O11" s="2">
+        <v>20.0621815110851</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="N12" s="3">
+        <f>SUM(N2:N11)</f>
+        <v>99.999999999999773</v>
+      </c>
+      <c r="O12" s="3">
+        <f>SUM(O2:O11)</f>
+        <v>99.999999999999787</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="N2:N11">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O2:O11">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FCC801C-C42A-5A46-B8CE-335E1DD1C035}">
+  <dimension ref="A1:S12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="16.33203125" customWidth="1"/>
+    <col min="8" max="15" width="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.33203125" customWidth="1"/>
+    <col min="19" max="19" width="10.83203125" style="21"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P1" s="22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2747642.50515944</v>
+      </c>
+      <c r="C3" s="3">
+        <v>32807166219.147499</v>
+      </c>
+      <c r="D3" s="3">
+        <v>29276373226.599098</v>
+      </c>
+      <c r="E3" s="3">
+        <v>12730887016.797501</v>
+      </c>
+      <c r="F3" s="3">
+        <v>16287403643.337299</v>
+      </c>
+      <c r="G3" s="3">
+        <v>29018290660.1348</v>
+      </c>
+      <c r="H3" s="3">
+        <v>43.871939825480901</v>
+      </c>
+      <c r="I3" s="3">
+        <v>56.128060174519</v>
+      </c>
+      <c r="J3" s="3">
+        <v>38.805201679891702</v>
+      </c>
+      <c r="K3" s="3">
+        <v>49.645871681021198</v>
+      </c>
+      <c r="L3" s="3">
+        <v>43.485191687715101</v>
+      </c>
+      <c r="M3" s="3">
+        <v>55.633269590030203</v>
+      </c>
+      <c r="N3" s="3">
+        <v>4.5101528767221497</v>
+      </c>
+      <c r="O3" s="3">
+        <v>5.5347405121886402</v>
+      </c>
+      <c r="P3" s="3">
+        <v>1527706442.0157001</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>1954488437.20047</v>
+      </c>
+      <c r="R3" s="24">
+        <v>5.2646327790577097</v>
+      </c>
+      <c r="S3" s="23">
+        <f>P3/G3</f>
+        <v>5.2646327790577152E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
+        <v>2748295.6540946802</v>
+      </c>
+      <c r="C4" s="3">
+        <v>41822410674.936996</v>
+      </c>
+      <c r="D4" s="3">
+        <v>35426039310.566101</v>
+      </c>
+      <c r="E4" s="3">
+        <v>16171881744.9347</v>
+      </c>
+      <c r="F4" s="3">
+        <v>18893257154.780602</v>
+      </c>
+      <c r="G4" s="3">
+        <v>35065138899.715302</v>
+      </c>
+      <c r="H4" s="3">
+        <v>46.119542806277003</v>
+      </c>
+      <c r="I4" s="3">
+        <v>53.880457193722897</v>
+      </c>
+      <c r="J4" s="3">
+        <v>38.667980835992402</v>
+      </c>
+      <c r="K4" s="3">
+        <v>45.174959668460197</v>
+      </c>
+      <c r="L4" s="3">
+        <v>45.649703042336199</v>
+      </c>
+      <c r="M4" s="3">
+        <v>53.331553632487299</v>
+      </c>
+      <c r="N4" s="3">
+        <v>5.7291890877431797</v>
+      </c>
+      <c r="O4" s="3">
+        <v>6.4202544537869501</v>
+      </c>
+      <c r="P4" s="3">
+        <v>1940625809.3921599</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>2267190858.5736699</v>
+      </c>
+      <c r="R4" s="24">
+        <v>5.5343451367532399</v>
+      </c>
+      <c r="S4" s="23">
+        <f t="shared" ref="S4:S12" si="0">P4/G4</f>
+        <v>5.5343451367532333E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3">
+        <v>2747874.69444041</v>
+      </c>
+      <c r="C5" s="3">
+        <v>47728594014.963997</v>
+      </c>
+      <c r="D5" s="3">
+        <v>39497871055.729301</v>
+      </c>
+      <c r="E5" s="3">
+        <v>18492395560.589802</v>
+      </c>
+      <c r="F5" s="3">
+        <v>20558976669.909401</v>
+      </c>
+      <c r="G5" s="3">
+        <v>39051372230.499298</v>
+      </c>
+      <c r="H5" s="3">
+        <v>47.354022418057802</v>
+      </c>
+      <c r="I5" s="3">
+        <v>52.645977581942098</v>
+      </c>
+      <c r="J5" s="3">
+        <v>38.744899032207101</v>
+      </c>
+      <c r="K5" s="3">
+        <v>43.074758630986999</v>
+      </c>
+      <c r="L5" s="3">
+        <v>46.8187146960353</v>
+      </c>
+      <c r="M5" s="3">
+        <v>52.050847603664103</v>
+      </c>
+      <c r="N5" s="3">
+        <v>6.5512741512066697</v>
+      </c>
+      <c r="O5" s="3">
+        <v>6.9862946578742502</v>
+      </c>
+      <c r="P5" s="3">
+        <v>2219087467.2707801</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>2467077200.3891301</v>
+      </c>
+      <c r="R5" s="24">
+        <v>5.6824826901669301</v>
+      </c>
+      <c r="S5" s="23">
+        <f t="shared" si="0"/>
+        <v>5.6824826901669352E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3">
+        <v>2747979.4784429399</v>
+      </c>
+      <c r="C6" s="3">
+        <v>55228987672.520798</v>
+      </c>
+      <c r="D6" s="3">
+        <v>44792749154.822098</v>
+      </c>
+      <c r="E6" s="3">
+        <v>21174220742.446899</v>
+      </c>
+      <c r="F6" s="3">
+        <v>23060388456.8377</v>
+      </c>
+      <c r="G6" s="3">
+        <v>44234609199.284698</v>
+      </c>
+      <c r="H6" s="3">
+        <v>47.867995503370103</v>
+      </c>
+      <c r="I6" s="3">
+        <v>52.132004496629797</v>
+      </c>
+      <c r="J6" s="3">
+        <v>38.338962263800802</v>
+      </c>
+      <c r="K6" s="3">
+        <v>41.754139318239503</v>
+      </c>
+      <c r="L6" s="3">
+        <v>47.271536447249801</v>
+      </c>
+      <c r="M6" s="3">
+        <v>51.4824137655215</v>
+      </c>
+      <c r="N6" s="3">
+        <v>7.5013604682763004</v>
+      </c>
+      <c r="O6" s="3">
+        <v>7.8363175011677102</v>
+      </c>
+      <c r="P6" s="3">
+        <v>2540906489.0936298</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>2767246614.8205199</v>
+      </c>
+      <c r="R6" s="24">
+        <v>5.7441594604044202</v>
+      </c>
+      <c r="S6" s="23">
+        <f t="shared" si="0"/>
+        <v>5.7441594604044063E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3">
+        <v>2747628.8515828899</v>
+      </c>
+      <c r="C7" s="3">
+        <v>62300009849.796898</v>
+      </c>
+      <c r="D7" s="3">
+        <v>49501029635.587097</v>
+      </c>
+      <c r="E7" s="3">
+        <v>23802239836.017101</v>
+      </c>
+      <c r="F7" s="3">
+        <v>25029174922.970699</v>
+      </c>
+      <c r="G7" s="3">
+        <v>48831414758.9879</v>
+      </c>
+      <c r="H7" s="3">
+        <v>48.743703113037597</v>
+      </c>
+      <c r="I7" s="3">
+        <v>51.256296886962197</v>
+      </c>
+      <c r="J7" s="3">
+        <v>38.205836392969204</v>
+      </c>
+      <c r="K7" s="3">
+        <v>40.175234295010902</v>
+      </c>
+      <c r="L7" s="3">
+        <v>48.084332813362899</v>
+      </c>
+      <c r="M7" s="3">
+        <v>50.5629379979136</v>
+      </c>
+      <c r="N7" s="3">
+        <v>8.43238498049665</v>
+      </c>
+      <c r="O7" s="3">
+        <v>8.5053450793239804</v>
+      </c>
+      <c r="P7" s="3">
+        <v>2856268780.3220501</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>3003500990.7564902</v>
+      </c>
+      <c r="R7" s="24">
+        <v>5.8492443735645203</v>
+      </c>
+      <c r="S7" s="23">
+        <f t="shared" si="0"/>
+        <v>5.8492443735645112E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3">
+        <v>2748336.9317767601</v>
+      </c>
+      <c r="C8" s="3">
+        <v>70697712578.309692</v>
+      </c>
+      <c r="D8" s="3">
+        <v>54853430904.834999</v>
+      </c>
+      <c r="E8" s="3">
+        <v>26514380477.310398</v>
+      </c>
+      <c r="F8" s="3">
+        <v>27502940702.588501</v>
+      </c>
+      <c r="G8" s="3">
+        <v>54017321179.898903</v>
+      </c>
+      <c r="H8" s="3">
+        <v>49.084959968686903</v>
+      </c>
+      <c r="I8" s="3">
+        <v>50.915040031313097</v>
+      </c>
+      <c r="J8" s="3">
+        <v>37.503873195248303</v>
+      </c>
+      <c r="K8" s="3">
+        <v>38.902164864420897</v>
+      </c>
+      <c r="L8" s="3">
+        <v>48.336776824972098</v>
+      </c>
+      <c r="M8" s="3">
+        <v>50.138961681910502</v>
+      </c>
+      <c r="N8" s="3">
+        <v>9.39321111140681</v>
+      </c>
+      <c r="O8" s="3">
+        <v>9.3459733327851708</v>
+      </c>
+      <c r="P8" s="3">
+        <v>3181725657.2772498</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>3300352884.3106198</v>
+      </c>
+      <c r="R8" s="24">
+        <v>5.8901951962424297</v>
+      </c>
+      <c r="S8" s="23">
+        <f t="shared" si="0"/>
+        <v>5.8901951962424301E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3">
+        <v>2747846.3569293302</v>
+      </c>
+      <c r="C9" s="3">
+        <v>80541995781.497406</v>
+      </c>
+      <c r="D9" s="3">
+        <v>60962714759.237099</v>
+      </c>
+      <c r="E9" s="3">
+        <v>29742875498.603001</v>
+      </c>
+      <c r="F9" s="3">
+        <v>30134718319.903301</v>
+      </c>
+      <c r="G9" s="3">
+        <v>59877593818.506302</v>
+      </c>
+      <c r="H9" s="3">
+        <v>49.672796787319001</v>
+      </c>
+      <c r="I9" s="3">
+        <v>50.327203212680899</v>
+      </c>
+      <c r="J9" s="3">
+        <v>36.928406367396803</v>
+      </c>
+      <c r="K9" s="3">
+        <v>37.414913831606398</v>
+      </c>
+      <c r="L9" s="3">
+        <v>48.788633537840099</v>
+      </c>
+      <c r="M9" s="3">
+        <v>49.431391693949003</v>
+      </c>
+      <c r="N9" s="3">
+        <v>10.5369653595243</v>
+      </c>
+      <c r="O9" s="3">
+        <v>10.240296732425501</v>
+      </c>
+      <c r="P9" s="3">
+        <v>3569145059.8323598</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>3616166198.3884001</v>
+      </c>
+      <c r="R9" s="24">
+        <v>5.9607356144782901</v>
+      </c>
+      <c r="S9" s="23">
+        <f t="shared" si="0"/>
+        <v>5.9607356144782957E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3">
+        <v>2747984.4327531499</v>
+      </c>
+      <c r="C10" s="3">
+        <v>95316514865.332199</v>
+      </c>
+      <c r="D10" s="3">
+        <v>69592985603.748001</v>
+      </c>
+      <c r="E10" s="3">
+        <v>33989743428.753101</v>
+      </c>
+      <c r="F10" s="3">
+        <v>34113196809.400902</v>
+      </c>
+      <c r="G10" s="3">
+        <v>68102940238.154099</v>
+      </c>
+      <c r="H10" s="3">
+        <v>49.909362664654402</v>
+      </c>
+      <c r="I10" s="3">
+        <v>50.090637335345598</v>
+      </c>
+      <c r="J10" s="3">
+        <v>35.659868047814697</v>
+      </c>
+      <c r="K10" s="3">
+        <v>35.789387450430397</v>
+      </c>
+      <c r="L10" s="3">
+        <v>48.8407605075109</v>
+      </c>
+      <c r="M10" s="3">
+        <v>49.018153932403898</v>
+      </c>
+      <c r="N10" s="3">
+        <v>12.041497100867399</v>
+      </c>
+      <c r="O10" s="3">
+        <v>11.5922523021949</v>
+      </c>
+      <c r="P10" s="3">
+        <v>4078769211.4503798</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>4093583617.1281099</v>
+      </c>
+      <c r="R10" s="24">
+        <v>5.98912351975852</v>
+      </c>
+      <c r="S10" s="23">
+        <f t="shared" si="0"/>
+        <v>5.9891235197585255E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3">
+        <v>2748042.5822946099</v>
+      </c>
+      <c r="C11" s="3">
+        <v>117372854152.933</v>
+      </c>
+      <c r="D11" s="3">
+        <v>82061193028.969299</v>
+      </c>
+      <c r="E11" s="3">
+        <v>40088129768.291</v>
+      </c>
+      <c r="F11" s="3">
+        <v>39657623068.682297</v>
+      </c>
+      <c r="G11" s="3">
+        <v>79745752836.973297</v>
+      </c>
+      <c r="H11" s="3">
+        <v>50.269924531585197</v>
+      </c>
+      <c r="I11" s="3">
+        <v>49.730075468414697</v>
+      </c>
+      <c r="J11" s="3">
+        <v>34.154515588465898</v>
+      </c>
+      <c r="K11" s="3">
+        <v>33.7877300120943</v>
+      </c>
+      <c r="L11" s="3">
+        <v>48.851507379546597</v>
+      </c>
+      <c r="M11" s="3">
+        <v>48.326890707867697</v>
+      </c>
+      <c r="N11" s="3">
+        <v>14.2019635833945</v>
+      </c>
+      <c r="O11" s="3">
+        <v>13.4763439171676</v>
+      </c>
+      <c r="P11" s="3">
+        <v>4810575572.1949196</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>4758914768.2418804</v>
+      </c>
+      <c r="R11" s="24">
+        <v>6.0323909437902197</v>
+      </c>
+      <c r="S11" s="23">
+        <f t="shared" si="0"/>
+        <v>6.0323909437902327E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2748063.5193039002</v>
+      </c>
+      <c r="C12" s="3">
+        <v>205068163103.01001</v>
+      </c>
+      <c r="D12" s="3">
+        <v>124958992792.82401</v>
+      </c>
+      <c r="E12" s="3">
+        <v>59564986259.146202</v>
+      </c>
+      <c r="F12" s="3">
+        <v>59038151385.299301</v>
+      </c>
+      <c r="G12" s="3">
+        <v>118603137644.44501</v>
+      </c>
+      <c r="H12" s="3">
+        <v>50.222099888885801</v>
+      </c>
+      <c r="I12" s="3">
+        <v>49.7779001111141</v>
+      </c>
+      <c r="J12" s="3">
+        <v>29.046432833762299</v>
+      </c>
+      <c r="K12" s="3">
+        <v>28.7895256347729</v>
+      </c>
+      <c r="L12" s="3">
+        <v>47.667626737278198</v>
+      </c>
+      <c r="M12" s="3">
+        <v>47.246020527055002</v>
+      </c>
+      <c r="N12" s="3">
+        <v>21.102001280361801</v>
+      </c>
+      <c r="O12" s="3">
+        <v>20.0621815110851</v>
+      </c>
+      <c r="P12" s="3">
+        <v>7147798351.0975399</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>7084578166.23592</v>
+      </c>
+      <c r="R12" s="24">
+        <v>6.0266519866663</v>
+      </c>
+      <c r="S12" s="23">
+        <f t="shared" si="0"/>
+        <v>6.0266519866663239E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E37FD776-7F29-1443-8F72-00AEDE6040D3}">
+  <dimension ref="A1:M20"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="17.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.6640625" style="3" bestFit="1" customWidth="1"/>
@@ -2064,14 +3605,58 @@
         <v>6.0023082788553896</v>
       </c>
     </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="3">
+        <f>SUM(B3:B12)</f>
+        <v>27479695.00677811</v>
+      </c>
+      <c r="C13" s="3">
+        <f>SUM(C3:C12)</f>
+        <v>282271740332.88971</v>
+      </c>
+      <c r="D13" s="3">
+        <f>SUM(D3:D12)</f>
+        <v>294275831133.71002</v>
+      </c>
+      <c r="E13" s="3">
+        <f>SUM(E3:E12)</f>
+        <v>576547571466.59961</v>
+      </c>
+      <c r="F13" s="3">
+        <f>SUM(F3:F12)</f>
+        <v>33872608839.946754</v>
+      </c>
+      <c r="G13" s="3">
+        <f>SUM(G3:G12)</f>
+        <v>35313099736.045197</v>
+      </c>
+    </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="3">
+        <f>C13*12</f>
+        <v>3387260883994.6768</v>
+      </c>
+      <c r="D14" s="3">
+        <f>D13*12</f>
+        <v>3531309973604.5205</v>
+      </c>
+      <c r="E14" s="3">
+        <f>E13*12</f>
+        <v>6918570857599.1953</v>
+      </c>
       <c r="F14" s="3">
-        <f>C3*0.12</f>
-        <v>1527706442.0157001</v>
+        <f>F13*12</f>
+        <v>406471306079.36108</v>
       </c>
       <c r="G14" s="3">
-        <f>D3*0.12</f>
-        <v>1954488437.2004759</v>
+        <f>G13*12</f>
+        <v>423757196832.54236</v>
       </c>
       <c r="J14" s="8">
         <f>F3/E3</f>
@@ -2082,17 +3667,52 @@
         <v>5.1671901749533982</v>
       </c>
     </row>
-    <row r="18" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="3">
+        <f>C14/1000000000</f>
+        <v>3387.2608839946765</v>
+      </c>
+      <c r="D15" s="3">
+        <f>D14/1000000000</f>
+        <v>3531.3099736045206</v>
+      </c>
+      <c r="E15" s="3">
+        <f>E14/1000000000</f>
+        <v>6918.5708575991957</v>
+      </c>
+      <c r="F15" s="3">
+        <f>F14/1000000000</f>
+        <v>406.47130607936106</v>
+      </c>
+      <c r="G15" s="3">
+        <f>G14/1000000000</f>
+        <v>423.75719683254238</v>
+      </c>
+    </row>
+    <row r="17" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F17" s="3">
+        <f>C3*0.12</f>
+        <v>1527706442.0157001</v>
+      </c>
+      <c r="G17" s="3">
+        <f>D3*0.12</f>
+        <v>1954488437.2004759</v>
+      </c>
+    </row>
+    <row r="18" spans="6:9" x14ac:dyDescent="0.2">
       <c r="I18" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="6:9" x14ac:dyDescent="0.2">
       <c r="I19" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="6:9" x14ac:dyDescent="0.2">
       <c r="I20" s="3" t="s">
         <v>38</v>
       </c>
@@ -2100,4 +3720,1704 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D15D759-C211-6A47-BA8F-FA7924675BCB}">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.5" customWidth="1"/>
+    <col min="2" max="2" width="13" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="17.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="16.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="11" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>2747642.50515944</v>
+      </c>
+      <c r="C2" s="3">
+        <v>12730887016.797501</v>
+      </c>
+      <c r="D2" s="3">
+        <v>16287403643.337299</v>
+      </c>
+      <c r="E2" s="3">
+        <v>29018290660.1348</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1527706442.0157001</v>
+      </c>
+      <c r="G2" s="3">
+        <v>1954488437.20047</v>
+      </c>
+      <c r="H2" s="10">
+        <v>5.2096450668530103</v>
+      </c>
+      <c r="I2" s="10">
+        <v>6.7903549331469799</v>
+      </c>
+      <c r="J2" s="24">
+        <v>5.2646327790577203</v>
+      </c>
+      <c r="K2" s="10">
+        <v>6.7353672209422699</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2748295.6540946802</v>
+      </c>
+      <c r="C3" s="3">
+        <v>16171881744.9347</v>
+      </c>
+      <c r="D3" s="3">
+        <v>18893257154.780602</v>
+      </c>
+      <c r="E3" s="3">
+        <v>35065138899.715302</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1940625809.3921599</v>
+      </c>
+      <c r="G3" s="3">
+        <v>2267190858.5736699</v>
+      </c>
+      <c r="H3" s="10">
+        <v>5.45557234683627</v>
+      </c>
+      <c r="I3" s="10">
+        <v>6.5444276531637202</v>
+      </c>
+      <c r="J3" s="24">
+        <v>5.5343451367532399</v>
+      </c>
+      <c r="K3" s="10">
+        <v>6.4656548632467503</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>2747874.69444041</v>
+      </c>
+      <c r="C4" s="3">
+        <v>18492395560.589802</v>
+      </c>
+      <c r="D4" s="3">
+        <v>20558976669.909401</v>
+      </c>
+      <c r="E4" s="3">
+        <v>39051372230.499298</v>
+      </c>
+      <c r="F4" s="3">
+        <v>2219087467.2707801</v>
+      </c>
+      <c r="G4" s="3">
+        <v>2467077200.3891301</v>
+      </c>
+      <c r="H4" s="10">
+        <v>5.5568015023697797</v>
+      </c>
+      <c r="I4" s="10">
+        <v>6.4431984976302097</v>
+      </c>
+      <c r="J4" s="24">
+        <v>5.6824826901669301</v>
+      </c>
+      <c r="K4" s="10">
+        <v>6.3175173098330504</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>2747979.4784429399</v>
+      </c>
+      <c r="C5" s="3">
+        <v>21174220742.446899</v>
+      </c>
+      <c r="D5" s="3">
+        <v>23060388456.8377</v>
+      </c>
+      <c r="E5" s="3">
+        <v>44234609199.284698</v>
+      </c>
+      <c r="F5" s="3">
+        <v>2540906489.0936298</v>
+      </c>
+      <c r="G5" s="3">
+        <v>2767246614.8205199</v>
+      </c>
+      <c r="H5" s="10">
+        <v>5.6050850955508604</v>
+      </c>
+      <c r="I5" s="10">
+        <v>6.3949149044491298</v>
+      </c>
+      <c r="J5" s="24">
+        <v>5.7441594604044202</v>
+      </c>
+      <c r="K5" s="10">
+        <v>6.2558405395955798</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>2747628.8515828899</v>
+      </c>
+      <c r="C6" s="3">
+        <v>23802239836.017101</v>
+      </c>
+      <c r="D6" s="3">
+        <v>25029174922.970699</v>
+      </c>
+      <c r="E6" s="3">
+        <v>48831414758.9879</v>
+      </c>
+      <c r="F6" s="3">
+        <v>2856268780.3220501</v>
+      </c>
+      <c r="G6" s="3">
+        <v>3003500990.7564902</v>
+      </c>
+      <c r="H6" s="10">
+        <v>5.6657757606204502</v>
+      </c>
+      <c r="I6" s="10">
+        <v>6.3342242393795303</v>
+      </c>
+      <c r="J6" s="24">
+        <v>5.8492443735645203</v>
+      </c>
+      <c r="K6" s="10">
+        <v>6.1507556264354699</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>2748336.9317767601</v>
+      </c>
+      <c r="C7" s="3">
+        <v>26514380477.310398</v>
+      </c>
+      <c r="D7" s="3">
+        <v>27502940702.588501</v>
+      </c>
+      <c r="E7" s="3">
+        <v>54017321179.898903</v>
+      </c>
+      <c r="F7" s="3">
+        <v>3181725657.2772498</v>
+      </c>
+      <c r="G7" s="3">
+        <v>3300352884.3106198</v>
+      </c>
+      <c r="H7" s="10">
+        <v>5.7076454835129597</v>
+      </c>
+      <c r="I7" s="10">
+        <v>6.2923545164870198</v>
+      </c>
+      <c r="J7" s="24">
+        <v>5.8901951962424297</v>
+      </c>
+      <c r="K7" s="10">
+        <v>6.1098048037575703</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>2747846.3569293302</v>
+      </c>
+      <c r="C8" s="3">
+        <v>29742875498.603001</v>
+      </c>
+      <c r="D8" s="3">
+        <v>30134718319.903301</v>
+      </c>
+      <c r="E8" s="3">
+        <v>59877593818.506302</v>
+      </c>
+      <c r="F8" s="3">
+        <v>3569145059.8323498</v>
+      </c>
+      <c r="G8" s="3">
+        <v>3616166198.3884001</v>
+      </c>
+      <c r="H8" s="10">
+        <v>5.7836230768009598</v>
+      </c>
+      <c r="I8" s="10">
+        <v>6.2163769231990296</v>
+      </c>
+      <c r="J8" s="24">
+        <v>5.9607356144782804</v>
+      </c>
+      <c r="K8" s="10">
+        <v>6.0392643855217099</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>2747984.4327531499</v>
+      </c>
+      <c r="C9" s="3">
+        <v>33989743428.753101</v>
+      </c>
+      <c r="D9" s="3">
+        <v>34113196809.400902</v>
+      </c>
+      <c r="E9" s="3">
+        <v>68102940238.154099</v>
+      </c>
+      <c r="F9" s="3">
+        <v>4078769211.4503798</v>
+      </c>
+      <c r="G9" s="3">
+        <v>4093583617.1281099</v>
+      </c>
+      <c r="H9" s="10">
+        <v>5.8240673550235202</v>
+      </c>
+      <c r="I9" s="10">
+        <v>6.17593264497647</v>
+      </c>
+      <c r="J9" s="24">
+        <v>5.9891235197585297</v>
+      </c>
+      <c r="K9" s="10">
+        <v>6.0108764802414703</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <v>2748042.5822946099</v>
+      </c>
+      <c r="C10" s="3">
+        <v>40088129768.291</v>
+      </c>
+      <c r="D10" s="3">
+        <v>39657623068.682297</v>
+      </c>
+      <c r="E10" s="3">
+        <v>79745752836.973297</v>
+      </c>
+      <c r="F10" s="3">
+        <v>4810575572.1949196</v>
+      </c>
+      <c r="G10" s="3">
+        <v>4758914768.2418804</v>
+      </c>
+      <c r="H10" s="10">
+        <v>5.8886923759085601</v>
+      </c>
+      <c r="I10" s="10">
+        <v>6.1113076240914399</v>
+      </c>
+      <c r="J10" s="24">
+        <v>6.0323909437902303</v>
+      </c>
+      <c r="K10" s="10">
+        <v>5.9676090562097599</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3">
+        <v>2748063.5193039002</v>
+      </c>
+      <c r="C11" s="3">
+        <v>59564986259.146202</v>
+      </c>
+      <c r="D11" s="3">
+        <v>59038151385.299301</v>
+      </c>
+      <c r="E11" s="3">
+        <v>118603137644.44501</v>
+      </c>
+      <c r="F11" s="3">
+        <v>7147798351.0975399</v>
+      </c>
+      <c r="G11" s="3">
+        <v>7084578166.2359104</v>
+      </c>
+      <c r="H11" s="10">
+        <v>5.9839345361788396</v>
+      </c>
+      <c r="I11" s="10">
+        <v>6.0160654638211497</v>
+      </c>
+      <c r="J11" s="24">
+        <v>6.0266519866663</v>
+      </c>
+      <c r="K11" s="10">
+        <v>5.9733480133336903</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="K2:K11">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57170206-C385-FB4D-AE0F-9F5493A369BC}">
+  <dimension ref="A1:W23"/>
+  <sheetViews>
+    <sheetView topLeftCell="F1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="Q24" sqref="Q24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="21" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" s="4" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>2747642.50515944</v>
+      </c>
+      <c r="C2" s="3">
+        <v>12730887016.797501</v>
+      </c>
+      <c r="D2" s="3">
+        <v>16287403643.337299</v>
+      </c>
+      <c r="E2" s="3">
+        <v>29018290660.1348</v>
+      </c>
+      <c r="F2" s="3">
+        <v>11749966829.580099</v>
+      </c>
+      <c r="G2" s="3">
+        <v>2812553619.8122001</v>
+      </c>
+      <c r="H2" s="3">
+        <v>682368.05463735096</v>
+      </c>
+      <c r="I2" s="3">
+        <v>146439152.57548499</v>
+      </c>
+      <c r="J2" s="3">
+        <v>740245419.25953496</v>
+      </c>
+      <c r="K2" s="3">
+        <v>18722509.991712101</v>
+      </c>
+      <c r="L2" s="3">
+        <v>706737356.34813797</v>
+      </c>
+      <c r="M2" s="3">
+        <v>112056387.715506</v>
+      </c>
+      <c r="N2" s="2">
+        <v>40.4915884508736</v>
+      </c>
+      <c r="O2" s="2">
+        <v>9.6923476739312999</v>
+      </c>
+      <c r="P2" s="2">
+        <v>2.35151016518965E-3</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>0.50464430965488405</v>
+      </c>
+      <c r="R2" s="2">
+        <v>2.5509614881502198</v>
+      </c>
+      <c r="S2" s="2">
+        <v>6.4519685914625494E-2</v>
+      </c>
+      <c r="T2" s="2">
+        <v>2.4354892733879998</v>
+      </c>
+      <c r="U2" s="2">
+        <v>0.386157782441157</v>
+      </c>
+      <c r="V2" s="11">
+        <f>SUM(N2:U2)</f>
+        <v>56.128060174518986</v>
+      </c>
+      <c r="W2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2748295.6540946802</v>
+      </c>
+      <c r="C3" s="3">
+        <v>16171881744.9347</v>
+      </c>
+      <c r="D3" s="3">
+        <v>18893257154.780602</v>
+      </c>
+      <c r="E3" s="3">
+        <v>35065138899.715302</v>
+      </c>
+      <c r="F3" s="3">
+        <v>12573505641.1355</v>
+      </c>
+      <c r="G3" s="3">
+        <v>3912457149.9829502</v>
+      </c>
+      <c r="H3" s="3">
+        <v>3514494.1785079702</v>
+      </c>
+      <c r="I3" s="3">
+        <v>245559719.78979</v>
+      </c>
+      <c r="J3" s="3">
+        <v>973711952.95135903</v>
+      </c>
+      <c r="K3" s="3">
+        <v>21590797.297966398</v>
+      </c>
+      <c r="L3" s="3">
+        <v>911750214.78615296</v>
+      </c>
+      <c r="M3" s="3">
+        <v>251167184.65831101</v>
+      </c>
+      <c r="N3" s="2">
+        <v>35.857566904540697</v>
+      </c>
+      <c r="O3" s="2">
+        <v>11.1576833081209</v>
+      </c>
+      <c r="P3" s="2">
+        <v>1.0022758468344399E-2</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>0.70029587075664901</v>
+      </c>
+      <c r="R3" s="2">
+        <v>2.7768660940888501</v>
+      </c>
+      <c r="S3" s="2">
+        <v>6.1573397326943599E-2</v>
+      </c>
+      <c r="T3" s="2">
+        <v>2.60016142355436</v>
+      </c>
+      <c r="U3" s="2">
+        <v>0.71628743686610497</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>2747874.69444041</v>
+      </c>
+      <c r="C4" s="3">
+        <v>18492395560.589802</v>
+      </c>
+      <c r="D4" s="3">
+        <v>20558976669.909401</v>
+      </c>
+      <c r="E4" s="3">
+        <v>39051372230.499298</v>
+      </c>
+      <c r="F4" s="3">
+        <v>12873701452.5397</v>
+      </c>
+      <c r="G4" s="3">
+        <v>4816495633.1432896</v>
+      </c>
+      <c r="H4" s="3">
+        <v>6545345.8693788797</v>
+      </c>
+      <c r="I4" s="3">
+        <v>297040768.76151502</v>
+      </c>
+      <c r="J4" s="3">
+        <v>1176231165.2918501</v>
+      </c>
+      <c r="K4" s="3">
+        <v>23549384.297754198</v>
+      </c>
+      <c r="L4" s="3">
+        <v>990002976.11519504</v>
+      </c>
+      <c r="M4" s="3">
+        <v>375409943.89073801</v>
+      </c>
+      <c r="N4" s="2">
+        <v>32.966066791592297</v>
+      </c>
+      <c r="O4" s="2">
+        <v>12.333742345119299</v>
+      </c>
+      <c r="P4" s="2">
+        <v>1.6760860106900199E-2</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>0.76064105253009495</v>
+      </c>
+      <c r="R4" s="2">
+        <v>3.0120098170921898</v>
+      </c>
+      <c r="S4" s="2">
+        <v>6.03036025437335E-2</v>
+      </c>
+      <c r="T4" s="2">
+        <v>2.5351298035616701</v>
+      </c>
+      <c r="U4" s="2">
+        <v>0.96132330939587596</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>2747979.4784429399</v>
+      </c>
+      <c r="C5" s="3">
+        <v>21174220742.446899</v>
+      </c>
+      <c r="D5" s="3">
+        <v>23060388456.8377</v>
+      </c>
+      <c r="E5" s="3">
+        <v>44234609199.284698</v>
+      </c>
+      <c r="F5" s="3">
+        <v>13497522993.0415</v>
+      </c>
+      <c r="G5" s="3">
+        <v>5883270171.1771803</v>
+      </c>
+      <c r="H5" s="3">
+        <v>20404872.510134902</v>
+      </c>
+      <c r="I5" s="3">
+        <v>446415780.096394</v>
+      </c>
+      <c r="J5" s="3">
+        <v>1431421145.7681899</v>
+      </c>
+      <c r="K5" s="3">
+        <v>28546724.8645088</v>
+      </c>
+      <c r="L5" s="3">
+        <v>1167293454.20645</v>
+      </c>
+      <c r="M5" s="3">
+        <v>585513315.17335296</v>
+      </c>
+      <c r="N5" s="2">
+        <v>30.513489860920401</v>
+      </c>
+      <c r="O5" s="2">
+        <v>13.300151798950001</v>
+      </c>
+      <c r="P5" s="2">
+        <v>4.61287504953585E-2</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>1.0092002352393601</v>
+      </c>
+      <c r="R5" s="2">
+        <v>3.2359755668223298</v>
+      </c>
+      <c r="S5" s="2">
+        <v>6.4534818734129196E-2</v>
+      </c>
+      <c r="T5" s="2">
+        <v>2.6388691464359701</v>
+      </c>
+      <c r="U5" s="2">
+        <v>1.3236543190322101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>2747628.8515828899</v>
+      </c>
+      <c r="C6" s="3">
+        <v>23802239836.017101</v>
+      </c>
+      <c r="D6" s="3">
+        <v>25029174922.970699</v>
+      </c>
+      <c r="E6" s="3">
+        <v>48831414758.9879</v>
+      </c>
+      <c r="F6" s="3">
+        <v>13949885494.784401</v>
+      </c>
+      <c r="G6" s="3">
+        <v>6807475547.4025803</v>
+      </c>
+      <c r="H6" s="3">
+        <v>29284980.175714001</v>
+      </c>
+      <c r="I6" s="3">
+        <v>586394502.75655198</v>
+      </c>
+      <c r="J6" s="3">
+        <v>1591829923.7634201</v>
+      </c>
+      <c r="K6" s="3">
+        <v>35019412.1843872</v>
+      </c>
+      <c r="L6" s="3">
+        <v>1258789933.1478701</v>
+      </c>
+      <c r="M6" s="3">
+        <v>770495128.75581396</v>
+      </c>
+      <c r="N6" s="2">
+        <v>28.5674407830193</v>
+      </c>
+      <c r="O6" s="2">
+        <v>13.9407706719158</v>
+      </c>
+      <c r="P6" s="2">
+        <v>5.9971598857523997E-2</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>1.20085503492118</v>
+      </c>
+      <c r="R6" s="2">
+        <v>3.2598480540038701</v>
+      </c>
+      <c r="S6" s="2">
+        <v>7.1714924413369602E-2</v>
+      </c>
+      <c r="T6" s="2">
+        <v>2.57782810381544</v>
+      </c>
+      <c r="U6" s="2">
+        <v>1.5778677160157299</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>2748336.9317767601</v>
+      </c>
+      <c r="C7" s="3">
+        <v>26514380477.310398</v>
+      </c>
+      <c r="D7" s="3">
+        <v>27502940702.588501</v>
+      </c>
+      <c r="E7" s="3">
+        <v>54017321179.898903</v>
+      </c>
+      <c r="F7" s="3">
+        <v>14397728035.304501</v>
+      </c>
+      <c r="G7" s="3">
+        <v>7927409860.6934099</v>
+      </c>
+      <c r="H7" s="3">
+        <v>63180521.006016403</v>
+      </c>
+      <c r="I7" s="3">
+        <v>683776655.87726998</v>
+      </c>
+      <c r="J7" s="3">
+        <v>1798324006.6226399</v>
+      </c>
+      <c r="K7" s="3">
+        <v>41077150.383075602</v>
+      </c>
+      <c r="L7" s="3">
+        <v>1510439607.86689</v>
+      </c>
+      <c r="M7" s="3">
+        <v>1081004864.8346601</v>
+      </c>
+      <c r="N7" s="2">
+        <v>26.653909747494598</v>
+      </c>
+      <c r="O7" s="2">
+        <v>14.675681221384499</v>
+      </c>
+      <c r="P7" s="2">
+        <v>0.116963447327571</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>1.2658470300665601</v>
+      </c>
+      <c r="R7" s="2">
+        <v>3.32916177133909</v>
+      </c>
+      <c r="S7" s="2">
+        <v>7.6044404805400395E-2</v>
+      </c>
+      <c r="T7" s="2">
+        <v>2.79621346426369</v>
+      </c>
+      <c r="U7" s="2">
+        <v>2.00121894463165</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>2747846.3569293302</v>
+      </c>
+      <c r="C8" s="3">
+        <v>29742875498.603001</v>
+      </c>
+      <c r="D8" s="3">
+        <v>30134718319.903301</v>
+      </c>
+      <c r="E8" s="3">
+        <v>59877593818.506302</v>
+      </c>
+      <c r="F8" s="3">
+        <v>14812993847.139601</v>
+      </c>
+      <c r="G8" s="3">
+        <v>9078634070.8402691</v>
+      </c>
+      <c r="H8" s="3">
+        <v>98781256.271991506</v>
+      </c>
+      <c r="I8" s="3">
+        <v>940093141.09905696</v>
+      </c>
+      <c r="J8" s="3">
+        <v>2005128937.83179</v>
+      </c>
+      <c r="K8" s="3">
+        <v>43262154.6866671</v>
+      </c>
+      <c r="L8" s="3">
+        <v>1698897899.0378699</v>
+      </c>
+      <c r="M8" s="3">
+        <v>1456927012.9960101</v>
+      </c>
+      <c r="N8" s="2">
+        <v>24.7387927645172</v>
+      </c>
+      <c r="O8" s="2">
+        <v>15.161988803956101</v>
+      </c>
+      <c r="P8" s="2">
+        <v>0.16497198696962501</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>1.5700249144088001</v>
+      </c>
+      <c r="R8" s="2">
+        <v>3.3487132831514499</v>
+      </c>
+      <c r="S8" s="2">
+        <v>7.2250990608938095E-2</v>
+      </c>
+      <c r="T8" s="2">
+        <v>2.8372848518051099</v>
+      </c>
+      <c r="U8" s="2">
+        <v>2.4331756172635601</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>2747984.4327531499</v>
+      </c>
+      <c r="C9" s="3">
+        <v>33989743428.753101</v>
+      </c>
+      <c r="D9" s="3">
+        <v>34113196809.400902</v>
+      </c>
+      <c r="E9" s="3">
+        <v>68102940238.154099</v>
+      </c>
+      <c r="F9" s="3">
+        <v>15354359285.5842</v>
+      </c>
+      <c r="G9" s="3">
+        <v>10607649334.290899</v>
+      </c>
+      <c r="H9" s="3">
+        <v>259129992.405334</v>
+      </c>
+      <c r="I9" s="3">
+        <v>1331883811.2451601</v>
+      </c>
+      <c r="J9" s="3">
+        <v>2229614217.6897001</v>
+      </c>
+      <c r="K9" s="3">
+        <v>56873922.294415303</v>
+      </c>
+      <c r="L9" s="3">
+        <v>2272578925.0672698</v>
+      </c>
+      <c r="M9" s="3">
+        <v>2001107320.8238399</v>
+      </c>
+      <c r="N9" s="2">
+        <v>22.545809669730001</v>
+      </c>
+      <c r="O9" s="2">
+        <v>15.5759050889672</v>
+      </c>
+      <c r="P9" s="2">
+        <v>0.380497510825764</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>1.9556920840533401</v>
+      </c>
+      <c r="R9" s="2">
+        <v>3.2738883371155501</v>
+      </c>
+      <c r="S9" s="2">
+        <v>8.3511698754163602E-2</v>
+      </c>
+      <c r="T9" s="2">
+        <v>3.3369762261660401</v>
+      </c>
+      <c r="U9" s="2">
+        <v>2.9383567197334202</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <v>2748042.5822946099</v>
+      </c>
+      <c r="C10" s="3">
+        <v>40088129768.291</v>
+      </c>
+      <c r="D10" s="3">
+        <v>39657623068.682297</v>
+      </c>
+      <c r="E10" s="3">
+        <v>79745752836.973297</v>
+      </c>
+      <c r="F10" s="3">
+        <v>15656353582.4806</v>
+      </c>
+      <c r="G10" s="3">
+        <v>13515157125.381001</v>
+      </c>
+      <c r="H10" s="3">
+        <v>588308177.40277696</v>
+      </c>
+      <c r="I10" s="3">
+        <v>1659423366.5900199</v>
+      </c>
+      <c r="J10" s="3">
+        <v>2290156689.4618702</v>
+      </c>
+      <c r="K10" s="3">
+        <v>73316810.959874198</v>
+      </c>
+      <c r="L10" s="3">
+        <v>2926009636.4663601</v>
+      </c>
+      <c r="M10" s="3">
+        <v>2948897679.9398398</v>
+      </c>
+      <c r="N10" s="2">
+        <v>19.632836891623999</v>
+      </c>
+      <c r="O10" s="2">
+        <v>16.947808058205201</v>
+      </c>
+      <c r="P10" s="2">
+        <v>0.73772979309064102</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>2.0808924708284202</v>
+      </c>
+      <c r="R10" s="2">
+        <v>2.8718227717326901</v>
+      </c>
+      <c r="S10" s="2">
+        <v>9.1938201536272302E-2</v>
+      </c>
+      <c r="T10" s="2">
+        <v>3.6691730059255798</v>
+      </c>
+      <c r="U10" s="2">
+        <v>3.6978742754719001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3">
+        <v>2748063.5193039002</v>
+      </c>
+      <c r="C11" s="3">
+        <v>59564986259.146202</v>
+      </c>
+      <c r="D11" s="3">
+        <v>59038151385.299301</v>
+      </c>
+      <c r="E11" s="3">
+        <v>118603137644.44501</v>
+      </c>
+      <c r="F11" s="3">
+        <v>16542862951.057899</v>
+      </c>
+      <c r="G11" s="3">
+        <v>23160110972.182598</v>
+      </c>
+      <c r="H11" s="3">
+        <v>3164214992.7171102</v>
+      </c>
+      <c r="I11" s="3">
+        <v>3337260493.5719199</v>
+      </c>
+      <c r="J11" s="3">
+        <v>2376970075.4717598</v>
+      </c>
+      <c r="K11" s="3">
+        <v>114666989.84030101</v>
+      </c>
+      <c r="L11" s="3">
+        <v>5048127232.1395798</v>
+      </c>
+      <c r="M11" s="3">
+        <v>5293937678.3180199</v>
+      </c>
+      <c r="N11" s="2">
+        <v>13.9480820487658</v>
+      </c>
+      <c r="O11" s="2">
+        <v>19.527401578205399</v>
+      </c>
+      <c r="P11" s="2">
+        <v>2.6679015880700798</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>2.8138045585071501</v>
+      </c>
+      <c r="R11" s="2">
+        <v>2.0041375992914801</v>
+      </c>
+      <c r="S11" s="2">
+        <v>9.6681244794767598E-2</v>
+      </c>
+      <c r="T11" s="2">
+        <v>4.2563184519393698</v>
+      </c>
+      <c r="U11" s="2">
+        <v>4.4635730415399699</v>
+      </c>
+      <c r="V11" s="11">
+        <f>SUM(N11:U11)</f>
+        <v>49.777900111114022</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="O13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14" s="12">
+        <f>F2/$D2</f>
+        <v>0.72141435718557068</v>
+      </c>
+      <c r="G14" s="9">
+        <f>G2/$D2</f>
+        <v>0.17268274805498135</v>
+      </c>
+      <c r="H14" s="9">
+        <f>H2/$D2</f>
+        <v>4.1895446909765005E-5</v>
+      </c>
+      <c r="I14" s="9">
+        <f>I2/$D2</f>
+        <v>8.9909451366356335E-3</v>
+      </c>
+      <c r="J14" s="9">
+        <f>J2/$D2</f>
+        <v>4.5448951562169194E-2</v>
+      </c>
+      <c r="K14" s="9">
+        <f>K2/$D2</f>
+        <v>1.1495085651279315E-3</v>
+      </c>
+      <c r="L14" s="9">
+        <f>L2/$D2</f>
+        <v>4.3391652336021255E-2</v>
+      </c>
+      <c r="M14" s="9">
+        <f>M2/$D2</f>
+        <v>6.8799417125850497E-3</v>
+      </c>
+      <c r="O14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15" s="9">
+        <f>F3/$D3</f>
+        <v>0.66550227618925939</v>
+      </c>
+      <c r="G15" s="9">
+        <f>G3/$D3</f>
+        <v>0.20708219434746711</v>
+      </c>
+      <c r="H15" s="9">
+        <f>H3/$D3</f>
+        <v>1.8601843767413552E-4</v>
+      </c>
+      <c r="I15" s="9">
+        <f>I3/$D3</f>
+        <v>1.2997214708828303E-2</v>
+      </c>
+      <c r="J15" s="9">
+        <f>J3/$D3</f>
+        <v>5.1537537703231794E-2</v>
+      </c>
+      <c r="K15" s="9">
+        <f>K3/$D3</f>
+        <v>1.14277792977074E-3</v>
+      </c>
+      <c r="L15" s="9">
+        <f>L3/$D3</f>
+        <v>4.8257968825425678E-2</v>
+      </c>
+      <c r="M15" s="9">
+        <f>M3/$D3</f>
+        <v>1.3294011858339505E-2</v>
+      </c>
+      <c r="O15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="E16">
+        <v>3</v>
+      </c>
+      <c r="F16" s="9">
+        <f>F4/$D4</f>
+        <v>0.6261839613535799</v>
+      </c>
+      <c r="G16" s="9">
+        <f>G4/$D4</f>
+        <v>0.23427701244453597</v>
+      </c>
+      <c r="H16" s="9">
+        <f>H4/$D4</f>
+        <v>3.1836924446530459E-4</v>
+      </c>
+      <c r="I16" s="9">
+        <f>I4/$D4</f>
+        <v>1.4448227337903975E-2</v>
+      </c>
+      <c r="J16" s="9">
+        <f>J4/$D4</f>
+        <v>5.7212534659539231E-2</v>
+      </c>
+      <c r="K16" s="9">
+        <f>K4/$D4</f>
+        <v>1.1454550815372844E-3</v>
+      </c>
+      <c r="L16" s="9">
+        <f>L4/$D4</f>
+        <v>4.8154292502514802E-2</v>
+      </c>
+      <c r="M16" s="9">
+        <f>M4/$D4</f>
+        <v>1.8260147375924445E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="5:15" x14ac:dyDescent="0.2">
+      <c r="E17">
+        <v>4</v>
+      </c>
+      <c r="F17" s="9">
+        <f>F5/$D5</f>
+        <v>0.58531203922713249</v>
+      </c>
+      <c r="G17" s="9">
+        <f>G5/$D5</f>
+        <v>0.25512450417688931</v>
+      </c>
+      <c r="H17" s="9">
+        <f>H5/$D5</f>
+        <v>8.8484513382447363E-4</v>
+      </c>
+      <c r="I17" s="9">
+        <f>I5/$D5</f>
+        <v>1.9358554212213455E-2</v>
+      </c>
+      <c r="J17" s="9">
+        <f>J5/$D5</f>
+        <v>6.2072724769896719E-2</v>
+      </c>
+      <c r="K17" s="9">
+        <f>K5/$D5</f>
+        <v>1.2379117081197447E-3</v>
+      </c>
+      <c r="L17" s="9">
+        <f>L5/$D5</f>
+        <v>5.0618984861910798E-2</v>
+      </c>
+      <c r="M17" s="9">
+        <f>M5/$D5</f>
+        <v>2.5390435910013508E-2</v>
+      </c>
+      <c r="O17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="5:15" x14ac:dyDescent="0.2">
+      <c r="E18">
+        <v>5</v>
+      </c>
+      <c r="F18" s="9">
+        <f>F6/$D6</f>
+        <v>0.55734499989377584</v>
+      </c>
+      <c r="G18" s="9">
+        <f>G6/$D6</f>
+        <v>0.27198162018337135</v>
+      </c>
+      <c r="H18" s="9">
+        <f>H6/$D6</f>
+        <v>1.1700337812109622E-3</v>
+      </c>
+      <c r="I18" s="9">
+        <f>I6/$D6</f>
+        <v>2.3428439193909838E-2</v>
+      </c>
+      <c r="J18" s="9">
+        <f>J6/$D6</f>
+        <v>6.359897714017361E-2</v>
+      </c>
+      <c r="K18" s="9">
+        <f>K6/$D6</f>
+        <v>1.3991436909990944E-3</v>
+      </c>
+      <c r="L18" s="9">
+        <f>L6/$D6</f>
+        <v>5.0292905659970709E-2</v>
+      </c>
+      <c r="M18" s="9">
+        <f>M6/$D6</f>
+        <v>3.0783880456590147E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="5:15" x14ac:dyDescent="0.2">
+      <c r="E19">
+        <v>6</v>
+      </c>
+      <c r="F19" s="9">
+        <f>F7/$D7</f>
+        <v>0.52349776669334225</v>
+      </c>
+      <c r="G19" s="9">
+        <f>G7/$D7</f>
+        <v>0.28823862678609141</v>
+      </c>
+      <c r="H19" s="9">
+        <f>H7/$D7</f>
+        <v>2.2972278378969864E-3</v>
+      </c>
+      <c r="I19" s="9">
+        <f>I7/$D7</f>
+        <v>2.4861947064915672E-2</v>
+      </c>
+      <c r="J19" s="9">
+        <f>J7/$D7</f>
+        <v>6.5386608147447539E-2</v>
+      </c>
+      <c r="K19" s="9">
+        <f>K7/$D7</f>
+        <v>1.4935548466353467E-3</v>
+      </c>
+      <c r="L19" s="9">
+        <f>L7/$D7</f>
+        <v>5.4919203884431583E-2</v>
+      </c>
+      <c r="M19" s="9">
+        <f>M7/$D7</f>
+        <v>3.9305064739237824E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="5:15" x14ac:dyDescent="0.2">
+      <c r="E20">
+        <v>7</v>
+      </c>
+      <c r="F20" s="9">
+        <f>F8/$D8</f>
+        <v>0.49155906120934112</v>
+      </c>
+      <c r="G20" s="9">
+        <f>G8/$D8</f>
+        <v>0.30126825724612916</v>
+      </c>
+      <c r="H20" s="9">
+        <f>H8/$D8</f>
+        <v>3.2779883728579176E-3</v>
+      </c>
+      <c r="I20" s="9">
+        <f>I8/$D8</f>
+        <v>3.1196347386401375E-2</v>
+      </c>
+      <c r="J20" s="9">
+        <f>J8/$D8</f>
+        <v>6.6538831275799501E-2</v>
+      </c>
+      <c r="K20" s="9">
+        <f>K8/$D8</f>
+        <v>1.4356249900001031E-3</v>
+      </c>
+      <c r="L20" s="9">
+        <f>L8/$D8</f>
+        <v>5.6376763870919819E-2</v>
+      </c>
+      <c r="M20" s="9">
+        <f>M8/$D8</f>
+        <v>4.8347125648549455E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="5:15" x14ac:dyDescent="0.2">
+      <c r="E21">
+        <v>8</v>
+      </c>
+      <c r="F21" s="9">
+        <f>F9/$D9</f>
+        <v>0.45010027560222238</v>
+      </c>
+      <c r="G21" s="9">
+        <f>G9/$D9</f>
+        <v>0.31095442017816538</v>
+      </c>
+      <c r="H21" s="9">
+        <f>H9/$D9</f>
+        <v>7.5961802657534298E-3</v>
+      </c>
+      <c r="I21" s="9">
+        <f>I9/$D9</f>
+        <v>3.9043066490857876E-2</v>
+      </c>
+      <c r="J21" s="9">
+        <f>J9/$D9</f>
+        <v>6.5359286910198461E-2</v>
+      </c>
+      <c r="K21" s="9">
+        <f>K9/$D9</f>
+        <v>1.6672117424873533E-3</v>
+      </c>
+      <c r="L21" s="9">
+        <f>L9/$D9</f>
+        <v>6.661876158264339E-2</v>
+      </c>
+      <c r="M21" s="9">
+        <f>M9/$D9</f>
+        <v>5.8660797227669252E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="5:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>9</v>
+      </c>
+      <c r="F22" s="9">
+        <f>F10/$D10</f>
+        <v>0.39478799713653173</v>
+      </c>
+      <c r="G22" s="9">
+        <f>G10/$D10</f>
+        <v>0.34079594487986214</v>
+      </c>
+      <c r="H22" s="9">
+        <f>H10/$D10</f>
+        <v>1.4834680746849023E-2</v>
+      </c>
+      <c r="I22" s="9">
+        <f>I10/$D10</f>
+        <v>4.184374246827894E-2</v>
+      </c>
+      <c r="J22" s="9">
+        <f>J10/$D10</f>
+        <v>5.7748208597766706E-2</v>
+      </c>
+      <c r="K22" s="9">
+        <f>K10/$D10</f>
+        <v>1.8487444603752015E-3</v>
+      </c>
+      <c r="L22" s="9">
+        <f>L10/$D10</f>
+        <v>7.3781770314344325E-2</v>
+      </c>
+      <c r="M22" s="9">
+        <f>M10/$D10</f>
+        <v>7.4358911395993127E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="5:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <v>10</v>
+      </c>
+      <c r="F23" s="12">
+        <f>F11/$D11</f>
+        <v>0.28020631681189678</v>
+      </c>
+      <c r="G23" s="12">
+        <f>G11/$D11</f>
+        <v>0.39229058547299878</v>
+      </c>
+      <c r="H23" s="9">
+        <f>H11/$D11</f>
+        <v>5.359610554311852E-2</v>
+      </c>
+      <c r="I23" s="9">
+        <f>I11/$D11</f>
+        <v>5.6527184799402594E-2</v>
+      </c>
+      <c r="J23" s="9">
+        <f>J11/$D11</f>
+        <v>4.0261593896444958E-2</v>
+      </c>
+      <c r="K23" s="9">
+        <f>K11/$D11</f>
+        <v>1.9422523766361268E-3</v>
+      </c>
+      <c r="L23" s="13">
+        <f>L11/$D11</f>
+        <v>8.5506187332901148E-2</v>
+      </c>
+      <c r="M23" s="14">
+        <f>M11/$D11</f>
+        <v>8.966977376659914E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="N2:U2">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N11:U11">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N3:U3">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N4:U4">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N5:U5">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N6:U6">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N7:U7">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N8:U8">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N9:U9">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N10:U10">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F14:M14">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F15:M23">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added small multiples for exempt categories
</commit_message>
<xml_diff>
--- a/outputs/tax_share_sum.xlsx
+++ b/outputs/tax_share_sum.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11130"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edreiyu/Documents/Projects/vat_burden_analysis/outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A3E632-A166-614F-A7D0-A63F82CC1DDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{386635D1-3098-D748-A4E1-C9044719D7AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="460" yWindow="540" windowWidth="24900" windowHeight="19480" activeTab="6" xr2:uid="{EE8D4940-C3F8-D340-AF33-192918B31EA6}"/>
+    <workbookView xWindow="460" yWindow="500" windowWidth="36860" windowHeight="19480" activeTab="4" xr2:uid="{EE8D4940-C3F8-D340-AF33-192918B31EA6}"/>
   </bookViews>
   <sheets>
     <sheet name="tax_share" sheetId="1" r:id="rId1"/>
@@ -433,19 +433,6 @@
     <t>SHARE OF TOTAL EXEMPT SPENDING</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Share of spending on exempt goods/services </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Narrow (Body)"/>
-      </rPr>
-      <t>to total HH expenditures</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">A REDUCTION IN VAT RATE DOES NOT BENEFIT THE POOR (RELATIVE TO RICHER HH) </t>
   </si>
   <si>
@@ -462,6 +449,9 @@
   </si>
   <si>
     <t>weighted_number_seniors</t>
+  </si>
+  <si>
+    <t>Breakdown of the total HH spending on VAT exempt goods/services</t>
   </si>
 </sst>
 </file>
@@ -474,7 +464,7 @@
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -621,11 +611,6 @@
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Aptos Narrow (Body)"/>
     </font>
     <font>
       <sz val="14"/>
@@ -1025,7 +1010,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -1083,7 +1068,7 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1092,6 +1077,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="21" builtinId="30" customBuiltin="1"/>
@@ -2100,7 +2088,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FD4DD6E-9753-F443-8851-2FA8C38B9693}">
   <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
@@ -3860,7 +3848,7 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4271,6 +4259,18 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="J2:J11">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="K2:K11">
     <cfRule type="colorScale" priority="2">
       <colorScale>
@@ -4283,18 +4283,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J11">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
@@ -4304,8 +4292,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57170206-C385-FB4D-AE0F-9F5493A369BC}">
   <dimension ref="A1:W24"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="S26" sqref="S26"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5053,12 +5041,12 @@
         <v>49.777900111114022</v>
       </c>
       <c r="W11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E13" t="s">
-        <v>102</v>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="E13" s="32" t="s">
+        <v>108</v>
       </c>
       <c r="O13" t="s">
         <v>63</v>
@@ -5101,35 +5089,35 @@
         <v>1</v>
       </c>
       <c r="F15" s="11">
-        <f>F2/$D2</f>
+        <f t="shared" ref="F15:M24" si="0">F2/$D2</f>
         <v>0.72141435718557068</v>
       </c>
       <c r="G15" s="9">
-        <f>G2/$D2</f>
+        <f t="shared" si="0"/>
         <v>0.17268274805498135</v>
       </c>
       <c r="H15" s="9">
-        <f>H2/$D2</f>
+        <f t="shared" si="0"/>
         <v>4.1895446909765005E-5</v>
       </c>
       <c r="I15" s="9">
-        <f>I2/$D2</f>
+        <f t="shared" si="0"/>
         <v>8.9909451366356335E-3</v>
       </c>
       <c r="J15" s="9">
-        <f>J2/$D2</f>
+        <f t="shared" si="0"/>
         <v>4.5448951562169194E-2</v>
       </c>
       <c r="K15" s="9">
-        <f>K2/$D2</f>
+        <f t="shared" si="0"/>
         <v>1.1495085651279315E-3</v>
       </c>
       <c r="L15" s="9">
-        <f>L2/$D2</f>
+        <f t="shared" si="0"/>
         <v>4.3391652336021255E-2</v>
       </c>
       <c r="M15" s="9">
-        <f>M2/$D2</f>
+        <f t="shared" si="0"/>
         <v>6.8799417125850497E-3</v>
       </c>
       <c r="O15" t="s">
@@ -5141,35 +5129,35 @@
         <v>2</v>
       </c>
       <c r="F16" s="9">
-        <f>F3/$D3</f>
+        <f t="shared" si="0"/>
         <v>0.66550227618925939</v>
       </c>
       <c r="G16" s="9">
-        <f>G3/$D3</f>
+        <f t="shared" si="0"/>
         <v>0.20708219434746711</v>
       </c>
       <c r="H16" s="9">
-        <f>H3/$D3</f>
+        <f t="shared" si="0"/>
         <v>1.8601843767413552E-4</v>
       </c>
       <c r="I16" s="9">
-        <f>I3/$D3</f>
+        <f t="shared" si="0"/>
         <v>1.2997214708828303E-2</v>
       </c>
       <c r="J16" s="9">
-        <f>J3/$D3</f>
+        <f t="shared" si="0"/>
         <v>5.1537537703231794E-2</v>
       </c>
       <c r="K16" s="9">
-        <f>K3/$D3</f>
+        <f t="shared" si="0"/>
         <v>1.14277792977074E-3</v>
       </c>
       <c r="L16" s="9">
-        <f>L3/$D3</f>
+        <f t="shared" si="0"/>
         <v>4.8257968825425678E-2</v>
       </c>
       <c r="M16" s="9">
-        <f>M3/$D3</f>
+        <f t="shared" si="0"/>
         <v>1.3294011858339505E-2</v>
       </c>
     </row>
@@ -5178,35 +5166,35 @@
         <v>3</v>
       </c>
       <c r="F17" s="9">
-        <f>F4/$D4</f>
+        <f t="shared" si="0"/>
         <v>0.6261839613535799</v>
       </c>
       <c r="G17" s="9">
-        <f>G4/$D4</f>
+        <f t="shared" si="0"/>
         <v>0.23427701244453597</v>
       </c>
       <c r="H17" s="9">
-        <f>H4/$D4</f>
+        <f t="shared" si="0"/>
         <v>3.1836924446530459E-4</v>
       </c>
       <c r="I17" s="9">
-        <f>I4/$D4</f>
+        <f t="shared" si="0"/>
         <v>1.4448227337903975E-2</v>
       </c>
       <c r="J17" s="9">
-        <f>J4/$D4</f>
+        <f t="shared" si="0"/>
         <v>5.7212534659539231E-2</v>
       </c>
       <c r="K17" s="9">
-        <f>K4/$D4</f>
+        <f t="shared" si="0"/>
         <v>1.1454550815372844E-3</v>
       </c>
       <c r="L17" s="9">
-        <f>L4/$D4</f>
+        <f t="shared" si="0"/>
         <v>4.8154292502514802E-2</v>
       </c>
       <c r="M17" s="9">
-        <f>M4/$D4</f>
+        <f t="shared" si="0"/>
         <v>1.8260147375924445E-2</v>
       </c>
       <c r="O17" t="s">
@@ -5218,35 +5206,35 @@
         <v>4</v>
       </c>
       <c r="F18" s="9">
-        <f>F5/$D5</f>
+        <f t="shared" si="0"/>
         <v>0.58531203922713249</v>
       </c>
       <c r="G18" s="9">
-        <f>G5/$D5</f>
+        <f t="shared" si="0"/>
         <v>0.25512450417688931</v>
       </c>
       <c r="H18" s="9">
-        <f>H5/$D5</f>
+        <f t="shared" si="0"/>
         <v>8.8484513382447363E-4</v>
       </c>
       <c r="I18" s="9">
-        <f>I5/$D5</f>
+        <f t="shared" si="0"/>
         <v>1.9358554212213455E-2</v>
       </c>
       <c r="J18" s="9">
-        <f>J5/$D5</f>
+        <f t="shared" si="0"/>
         <v>6.2072724769896719E-2</v>
       </c>
       <c r="K18" s="9">
-        <f>K5/$D5</f>
+        <f t="shared" si="0"/>
         <v>1.2379117081197447E-3</v>
       </c>
       <c r="L18" s="9">
-        <f>L5/$D5</f>
+        <f t="shared" si="0"/>
         <v>5.0618984861910798E-2</v>
       </c>
       <c r="M18" s="9">
-        <f>M5/$D5</f>
+        <f t="shared" si="0"/>
         <v>2.5390435910013508E-2</v>
       </c>
     </row>
@@ -5255,39 +5243,39 @@
         <v>5</v>
       </c>
       <c r="F19" s="9">
-        <f>F6/$D6</f>
+        <f t="shared" si="0"/>
         <v>0.55734499989377584</v>
       </c>
       <c r="G19" s="9">
-        <f>G6/$D6</f>
+        <f t="shared" si="0"/>
         <v>0.27198162018337135</v>
       </c>
       <c r="H19" s="9">
-        <f>H6/$D6</f>
+        <f t="shared" si="0"/>
         <v>1.1700337812109622E-3</v>
       </c>
       <c r="I19" s="9">
-        <f>I6/$D6</f>
+        <f t="shared" si="0"/>
         <v>2.3428439193909838E-2</v>
       </c>
       <c r="J19" s="9">
-        <f>J6/$D6</f>
+        <f t="shared" si="0"/>
         <v>6.359897714017361E-2</v>
       </c>
       <c r="K19" s="9">
-        <f>K6/$D6</f>
+        <f t="shared" si="0"/>
         <v>1.3991436909990944E-3</v>
       </c>
       <c r="L19" s="9">
-        <f>L6/$D6</f>
+        <f t="shared" si="0"/>
         <v>5.0292905659970709E-2</v>
       </c>
       <c r="M19" s="9">
-        <f>M6/$D6</f>
+        <f t="shared" si="0"/>
         <v>3.0783880456590147E-2</v>
       </c>
       <c r="O19" s="27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="P19" s="28"/>
       <c r="Q19" s="28"/>
@@ -5301,39 +5289,39 @@
         <v>6</v>
       </c>
       <c r="F20" s="9">
-        <f>F7/$D7</f>
+        <f t="shared" si="0"/>
         <v>0.52349776669334225</v>
       </c>
       <c r="G20" s="9">
-        <f>G7/$D7</f>
+        <f t="shared" si="0"/>
         <v>0.28823862678609141</v>
       </c>
       <c r="H20" s="9">
-        <f>H7/$D7</f>
+        <f t="shared" si="0"/>
         <v>2.2972278378969864E-3</v>
       </c>
       <c r="I20" s="9">
-        <f>I7/$D7</f>
+        <f t="shared" si="0"/>
         <v>2.4861947064915672E-2</v>
       </c>
       <c r="J20" s="9">
-        <f>J7/$D7</f>
+        <f t="shared" si="0"/>
         <v>6.5386608147447539E-2</v>
       </c>
       <c r="K20" s="9">
-        <f>K7/$D7</f>
+        <f t="shared" si="0"/>
         <v>1.4935548466353467E-3</v>
       </c>
       <c r="L20" s="9">
-        <f>L7/$D7</f>
+        <f t="shared" si="0"/>
         <v>5.4919203884431583E-2</v>
       </c>
       <c r="M20" s="9">
-        <f>M7/$D7</f>
+        <f t="shared" si="0"/>
         <v>3.9305064739237824E-2</v>
       </c>
       <c r="O20" s="27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="P20" s="28"/>
       <c r="Q20" s="28"/>
@@ -5347,35 +5335,35 @@
         <v>7</v>
       </c>
       <c r="F21" s="9">
-        <f>F8/$D8</f>
+        <f t="shared" si="0"/>
         <v>0.49155906120934112</v>
       </c>
       <c r="G21" s="9">
-        <f>G8/$D8</f>
+        <f t="shared" si="0"/>
         <v>0.30126825724612916</v>
       </c>
       <c r="H21" s="9">
-        <f>H8/$D8</f>
+        <f t="shared" si="0"/>
         <v>3.2779883728579176E-3</v>
       </c>
       <c r="I21" s="9">
-        <f>I8/$D8</f>
+        <f t="shared" si="0"/>
         <v>3.1196347386401375E-2</v>
       </c>
       <c r="J21" s="9">
-        <f>J8/$D8</f>
+        <f t="shared" si="0"/>
         <v>6.6538831275799501E-2</v>
       </c>
       <c r="K21" s="9">
-        <f>K8/$D8</f>
+        <f t="shared" si="0"/>
         <v>1.4356249900001031E-3</v>
       </c>
       <c r="L21" s="9">
-        <f>L8/$D8</f>
+        <f t="shared" si="0"/>
         <v>5.6376763870919819E-2</v>
       </c>
       <c r="M21" s="9">
-        <f>M8/$D8</f>
+        <f t="shared" si="0"/>
         <v>4.8347125648549455E-2</v>
       </c>
     </row>
@@ -5384,35 +5372,35 @@
         <v>8</v>
       </c>
       <c r="F22" s="9">
-        <f>F9/$D9</f>
+        <f t="shared" si="0"/>
         <v>0.45010027560222238</v>
       </c>
       <c r="G22" s="9">
-        <f>G9/$D9</f>
+        <f t="shared" si="0"/>
         <v>0.31095442017816538</v>
       </c>
       <c r="H22" s="9">
-        <f>H9/$D9</f>
+        <f t="shared" si="0"/>
         <v>7.5961802657534298E-3</v>
       </c>
       <c r="I22" s="9">
-        <f>I9/$D9</f>
+        <f t="shared" si="0"/>
         <v>3.9043066490857876E-2</v>
       </c>
       <c r="J22" s="9">
-        <f>J9/$D9</f>
+        <f t="shared" si="0"/>
         <v>6.5359286910198461E-2</v>
       </c>
       <c r="K22" s="9">
-        <f>K9/$D9</f>
+        <f t="shared" si="0"/>
         <v>1.6672117424873533E-3</v>
       </c>
       <c r="L22" s="9">
-        <f>L9/$D9</f>
+        <f t="shared" si="0"/>
         <v>6.661876158264339E-2</v>
       </c>
       <c r="M22" s="9">
-        <f>M9/$D9</f>
+        <f t="shared" si="0"/>
         <v>5.8660797227669252E-2</v>
       </c>
     </row>
@@ -5421,35 +5409,35 @@
         <v>9</v>
       </c>
       <c r="F23" s="9">
-        <f>F10/$D10</f>
+        <f t="shared" si="0"/>
         <v>0.39478799713653173</v>
       </c>
       <c r="G23" s="9">
-        <f>G10/$D10</f>
+        <f t="shared" si="0"/>
         <v>0.34079594487986214</v>
       </c>
       <c r="H23" s="9">
-        <f>H10/$D10</f>
+        <f t="shared" si="0"/>
         <v>1.4834680746849023E-2</v>
       </c>
       <c r="I23" s="9">
-        <f>I10/$D10</f>
+        <f t="shared" si="0"/>
         <v>4.184374246827894E-2</v>
       </c>
       <c r="J23" s="9">
-        <f>J10/$D10</f>
+        <f t="shared" si="0"/>
         <v>5.7748208597766706E-2</v>
       </c>
       <c r="K23" s="9">
-        <f>K10/$D10</f>
+        <f t="shared" si="0"/>
         <v>1.8487444603752015E-3</v>
       </c>
       <c r="L23" s="9">
-        <f>L10/$D10</f>
+        <f t="shared" si="0"/>
         <v>7.3781770314344325E-2</v>
       </c>
       <c r="M23" s="9">
-        <f>M10/$D10</f>
+        <f t="shared" si="0"/>
         <v>7.4358911395993127E-2</v>
       </c>
     </row>
@@ -5458,35 +5446,35 @@
         <v>10</v>
       </c>
       <c r="F24" s="11">
-        <f>F11/$D11</f>
+        <f t="shared" si="0"/>
         <v>0.28020631681189678</v>
       </c>
       <c r="G24" s="11">
-        <f>G11/$D11</f>
+        <f t="shared" si="0"/>
         <v>0.39229058547299878</v>
       </c>
       <c r="H24" s="9">
-        <f>H11/$D11</f>
+        <f t="shared" si="0"/>
         <v>5.359610554311852E-2</v>
       </c>
       <c r="I24" s="9">
-        <f>I11/$D11</f>
+        <f t="shared" si="0"/>
         <v>5.6527184799402594E-2</v>
       </c>
       <c r="J24" s="9">
-        <f>J11/$D11</f>
+        <f t="shared" si="0"/>
         <v>4.0261593896444958E-2</v>
       </c>
       <c r="K24" s="9">
-        <f>K11/$D11</f>
+        <f t="shared" si="0"/>
         <v>1.9422523766361268E-3</v>
       </c>
       <c r="L24" s="12">
-        <f>L11/$D11</f>
+        <f t="shared" si="0"/>
         <v>8.5506187332901148E-2</v>
       </c>
       <c r="M24" s="13">
-        <f>M11/$D11</f>
+        <f t="shared" si="0"/>
         <v>8.966977376659914E-2</v>
       </c>
     </row>
@@ -5643,7 +5631,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FCC801C-C42A-5A46-B8CE-335E1DD1C035}">
   <dimension ref="A1:S13"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
@@ -6339,8 +6327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EE975D7-106D-0144-9A73-131DDC957899}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6353,38 +6341,38 @@
     <col min="10" max="11" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="D1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="4" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>